<commit_message>
p2 - UnitQlearning, SplitQlearning
</commit_message>
<xml_diff>
--- a/p2/history_Rate.xlsx
+++ b/p2/history_Rate.xlsx
@@ -2477,7 +2477,7 @@
         <v>582</v>
       </c>
       <c r="F102" t="n">
-        <v>1502851</v>
+        <v>1502850</v>
       </c>
     </row>
     <row r="103">
@@ -9097,7 +9097,7 @@
         <v>784</v>
       </c>
       <c r="F433" t="n">
-        <v>873211</v>
+        <v>873210</v>
       </c>
     </row>
     <row r="434">

</xml_diff>